<commit_message>
added dimension layer to dxf, updated bom
</commit_message>
<xml_diff>
--- a/doc/My_WilsonII_BOM.xlsx
+++ b/doc/My_WilsonII_BOM.xlsx
@@ -1513,17 +1513,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1550,6 +1539,17 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2015,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2034,22 +2034,22 @@
   <sheetData>
     <row r="2" spans="1:11">
       <c r="D2" s="61"/>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="68"/>
       <c r="G2" s="59">
         <f>J95</f>
-        <v>470.23500000000013</v>
+        <v>468.67500000000007</v>
       </c>
       <c r="H2" s="62"/>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="73"/>
+      <c r="J2" s="68"/>
       <c r="K2" s="60">
         <f>K95</f>
-        <v>325.86000000000007</v>
+        <v>317.39999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2059,10 +2059,10 @@
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="79"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="11" t="s">
         <v>15</v>
       </c>
@@ -2086,19 +2086,19 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="78"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
@@ -2278,19 +2278,19 @@
       <c r="K13" s="64"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="78"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="73"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
@@ -2403,19 +2403,19 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="78"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="73"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="7" t="s">
@@ -2452,19 +2452,19 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="78"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="73"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
@@ -2482,10 +2482,12 @@
       <c r="E21" s="19"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="6">
+        <v>1</v>
+      </c>
       <c r="I21" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="26" t="str">
         <f>IF(E21&gt;0,SUM(B21*E21),"")</f>
@@ -2512,10 +2514,12 @@
       <c r="E22" s="19"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6">
+        <v>1</v>
+      </c>
       <c r="I22" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="26" t="str">
         <f>IF(E22&gt;0,SUM(B22*E22),"")</f>
@@ -2542,10 +2546,12 @@
       <c r="E23" s="19"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="6">
+        <v>2</v>
+      </c>
       <c r="I23" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23" s="26" t="str">
         <f>IF(E23&gt;0,SUM(B23*E23),"")</f>
@@ -2565,41 +2571,43 @@
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="16">
-        <v>8.4600000000000009</v>
+      <c r="E24" s="22">
+        <v>6.9</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>35</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="H24" s="16">
+        <v>1</v>
+      </c>
       <c r="I24" s="36">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="24">
         <f>IF(E24&gt;0,SUM(B24*E24),"")</f>
-        <v>8.4600000000000009</v>
+        <v>6.9</v>
       </c>
       <c r="K24" s="25">
         <f>IF(E24&gt;0,IF(H24&gt;0,SUM(J24-(H24*E24)),J24),"")</f>
-        <v>8.4600000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="78"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="72"/>
+      <c r="K25" s="73"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
@@ -3152,19 +3160,19 @@
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="69"/>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="70"/>
-      <c r="K43" s="71"/>
+      <c r="B43" s="79"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="79"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+      <c r="I43" s="80"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="81"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="39" t="s">
@@ -3801,19 +3809,19 @@
       </c>
     </row>
     <row r="65" spans="1:13">
-      <c r="A65" s="68" t="s">
+      <c r="A65" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="69"/>
-      <c r="C65" s="69"/>
-      <c r="D65" s="69"/>
-      <c r="E65" s="70"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="70"/>
-      <c r="H65" s="70"/>
-      <c r="I65" s="70"/>
-      <c r="J65" s="70"/>
-      <c r="K65" s="71"/>
+      <c r="B65" s="79"/>
+      <c r="C65" s="79"/>
+      <c r="D65" s="79"/>
+      <c r="E65" s="80"/>
+      <c r="F65" s="80"/>
+      <c r="G65" s="80"/>
+      <c r="H65" s="80"/>
+      <c r="I65" s="80"/>
+      <c r="J65" s="80"/>
+      <c r="K65" s="81"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="40" t="s">
@@ -3936,19 +3944,19 @@
       <c r="K70" s="53"/>
     </row>
     <row r="71" spans="1:13">
-      <c r="A71" s="68" t="s">
+      <c r="A71" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="69"/>
-      <c r="C71" s="69"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="70"/>
-      <c r="F71" s="70"/>
-      <c r="G71" s="70"/>
-      <c r="H71" s="70"/>
-      <c r="I71" s="70"/>
-      <c r="J71" s="70"/>
-      <c r="K71" s="71"/>
+      <c r="B71" s="79"/>
+      <c r="C71" s="79"/>
+      <c r="D71" s="79"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="80"/>
+      <c r="H71" s="80"/>
+      <c r="I71" s="80"/>
+      <c r="J71" s="80"/>
+      <c r="K71" s="81"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="39" t="s">
@@ -4508,11 +4516,11 @@
       <c r="B90" s="2">
         <v>2</v>
       </c>
-      <c r="C90" s="67" t="s">
+      <c r="C90" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="D90" s="67"/>
-      <c r="E90" s="67"/>
+      <c r="D90" s="77"/>
+      <c r="E90" s="77"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
@@ -4536,11 +4544,11 @@
       <c r="B91" s="2">
         <v>4</v>
       </c>
-      <c r="C91" s="67" t="s">
+      <c r="C91" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="D91" s="67"/>
-      <c r="E91" s="67"/>
+      <c r="D91" s="77"/>
+      <c r="E91" s="77"/>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6">
@@ -4655,15 +4663,20 @@
     <row r="95" spans="1:13">
       <c r="J95" s="31">
         <f>SUM(J7:J94)</f>
-        <v>470.23500000000013</v>
+        <v>468.67500000000007</v>
       </c>
       <c r="K95" s="57">
         <f>SUM(K7:K94)</f>
-        <v>325.86000000000007</v>
+        <v>317.39999999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A65:K65"/>
+    <mergeCell ref="A71:K71"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="A18:K18"/>
@@ -4672,11 +4685,6 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A14:K14"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A65:K65"/>
-    <mergeCell ref="A71:K71"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:I10">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">

</xml_diff>